<commit_message>
update readme and preprocessing files
</commit_message>
<xml_diff>
--- a/matlab/subject_data_info.xlsx
+++ b/matlab/subject_data_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/tuna28ng_upenn_edu/Documents/Documents/GitHub/AO_human_v_robot_main/matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="11_F25DC773A252ABDACC1048EAD9DC5C4E5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94C4DE44-F7B5-457F-8CDD-E5B86B6ED90A}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="11_F25DC773A252ABDACC1048EAD9DC5C4E5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{775F5E7F-E8DB-48A1-A6B3-DE5683A7319F}"/>
   <bookViews>
-    <workbookView xWindow="26490" yWindow="780" windowWidth="24165" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24470" yWindow="8130" windowWidth="13540" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>filepath_edf</t>
   </si>
@@ -85,13 +85,79 @@
   </si>
   <si>
     <t>Psychopy_603_2024-04-15T193304.857787_EPOCFLEX_126268_2024.04.15T19.33.04.04.00.edf</t>
+  </si>
+  <si>
+    <t>39, 73, 76, 81, 87, 89, 109, 112, 113, 114, 117, 118</t>
+  </si>
+  <si>
+    <t>bad_channel</t>
+  </si>
+  <si>
+    <t>bad_epoch</t>
+  </si>
+  <si>
+    <t>8, 16, 18, 24, 29, 50, 62, 66, 70, 71, 75, 76, 77, 78, 83, 85, 87, 88, 90, 91, 93, 95, 97, 98, 100, 101, 103, 105, 106, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119</t>
+  </si>
+  <si>
+    <t>25, 16</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>49, 53, 59, 64, 68, 72, 78, 80, 87, 117</t>
+  </si>
+  <si>
+    <t>20, 16, 18, 15, 19</t>
+  </si>
+  <si>
+    <t>14, 26, 33, 70, 71, 72, 76, 119</t>
+  </si>
+  <si>
+    <t>9, 31</t>
+  </si>
+  <si>
+    <t>28, 32, 34, 36, 41, 47, 48, 51, 74, 94, 96</t>
+  </si>
+  <si>
+    <t>8, 29, 38, 55, 61, 83, 96, 105, 110, 120</t>
+  </si>
+  <si>
+    <t>30, 18</t>
+  </si>
+  <si>
+    <t>23, 3, 32</t>
+  </si>
+  <si>
+    <t>25, 3, 32</t>
+  </si>
+  <si>
+    <t>33, 39, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 68, 69, 74, 105, 120</t>
+  </si>
+  <si>
+    <t>5, 8, 9, 16, 18, 20, 21, 50, 53, 58, 65, 66, 73, 80, 82, 90, 103, 113, 116, 117, 124, 128, 129, 139, 140</t>
+  </si>
+  <si>
+    <t>4, 31, 25</t>
+  </si>
+  <si>
+    <t>9, 40, 43, 52, 55, 77, 89, 93, 94, 100, 101, 110, 115, 139</t>
+  </si>
+  <si>
+    <t>9, 11, 23, 29, 37, 39, 47, 51, 52, 55, 57, 62, 65, 67, 70, 74, 80, 81, 91, 97, 99, 101, 114, 116, 117, 129, 133</t>
+  </si>
+  <si>
+    <t>25, 10</t>
+  </si>
+  <si>
+    <t>8, 27, 49, 53, 56, 60, 64, 65, 66, 67, 73, 74, 88, 91, 93, 94, 97, 98, 99, 100, 102, 104, 115, 116, 118, 119, 120, 122, 138</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +171,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -114,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,20 +196,168 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -150,6 +372,22 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{572F687B-FA80-4FDE-936A-EEC697B19E75}" name="Table2" displayName="Table2" ref="A1:G15" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G15" xr:uid="{572F687B-FA80-4FDE-936A-EEC697B19E75}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{EAA4733D-DC15-4633-B9D8-45890FF2CD17}" name="filepath_edf" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{D647B9E9-A4E2-4624-96EF-BC319FF750A4}" name="protocol" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{E8952D3C-9366-4FC4-99EF-EC9E02B83436}" name="subject_id" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7190C2FD-0C51-4D16-91D9-EAC2C407709A}" name="experiment" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{45F579EF-FF78-4F92-ABDF-F7844ACD56FA}" name="EDF_filename" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{379A8667-B611-4585-855C-C1F0AC067569}" name="bad_channel" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{ADF4D06C-56DE-448E-8F1E-6527686E8C73}" name="bad_epoch" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,23 +653,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="83.85546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,241 +687,328 @@
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C2" s="4">
         <v>601</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C3" s="4">
         <v>601</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C4" s="4">
         <v>602</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="F4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C5" s="4">
         <v>602</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C6" s="4">
         <v>603</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C7" s="4">
         <v>603</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C8" s="4">
         <v>605</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C9" s="4">
         <v>605</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="F9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C10" s="4">
         <v>606</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C11" s="4">
         <v>606</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C12" s="4">
         <v>607</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="F12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C13" s="4">
         <v>607</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="F13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C14" s="4">
         <v>608</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1">
-        <v>830126</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="F14" s="2">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2">
+        <v>830126</v>
+      </c>
+      <c r="C15" s="4">
         <v>608</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="F15" s="2">
+        <v>18</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add new utility functions and update analysis scripts
</commit_message>
<xml_diff>
--- a/matlab/subject_data_info.xlsx
+++ b/matlab/subject_data_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/tuna28ng_upenn_edu/Documents/Documents/GitHub/AO_human_v_robot_main/matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="11_F25DC773A252ABDACC1048EAD9DC5C4E5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{775F5E7F-E8DB-48A1-A6B3-DE5683A7319F}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="11_F25DC773A252ABDACC1048EAD9DC5C4E5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33FD6B3F-AC75-49DC-B408-5E72640E8566}"/>
   <bookViews>
-    <workbookView xWindow="24470" yWindow="8130" windowWidth="13540" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4410" yWindow="-21720" windowWidth="37710" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>filepath_edf</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>8, 27, 49, 53, 56, 60, 64, 65, 66, 67, 73, 74, 88, 91, 93, 94, 97, 98, 99, 100, 102, 104, 115, 116, 118, 119, 120, 122, 138</t>
+  </si>
+  <si>
+    <t>med_cond</t>
+  </si>
+  <si>
+    <t>healthy</t>
+  </si>
+  <si>
+    <t>stroke</t>
   </si>
 </sst>
 </file>
@@ -233,14 +242,30 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
-      <font>
-        <b/>
-      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -273,6 +298,59 @@
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -292,40 +370,6 @@
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -370,21 +414,18 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{572F687B-FA80-4FDE-936A-EEC697B19E75}" name="Table2" displayName="Table2" ref="A1:G15" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G15" xr:uid="{572F687B-FA80-4FDE-936A-EEC697B19E75}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EAA4733D-DC15-4633-B9D8-45890FF2CD17}" name="filepath_edf" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{D647B9E9-A4E2-4624-96EF-BC319FF750A4}" name="protocol" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E8952D3C-9366-4FC4-99EF-EC9E02B83436}" name="subject_id" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{7190C2FD-0C51-4D16-91D9-EAC2C407709A}" name="experiment" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{45F579EF-FF78-4F92-ABDF-F7844ACD56FA}" name="EDF_filename" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{379A8667-B611-4585-855C-C1F0AC067569}" name="bad_channel" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{ADF4D06C-56DE-448E-8F1E-6527686E8C73}" name="bad_epoch" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{572F687B-FA80-4FDE-936A-EEC697B19E75}" name="Table2" displayName="Table2" ref="A1:H15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H15" xr:uid="{572F687B-FA80-4FDE-936A-EEC697B19E75}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{EAA4733D-DC15-4633-B9D8-45890FF2CD17}" name="filepath_edf" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D647B9E9-A4E2-4624-96EF-BC319FF750A4}" name="protocol" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{E8952D3C-9366-4FC4-99EF-EC9E02B83436}" name="subject_id" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{B84B3FDE-B537-47AE-A08D-B54C6FD8A497}" name="med_cond" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{7190C2FD-0C51-4D16-91D9-EAC2C407709A}" name="experiment" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{45F579EF-FF78-4F92-ABDF-F7844ACD56FA}" name="EDF_filename" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{379A8667-B611-4585-855C-C1F0AC067569}" name="bad_channel" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{ADF4D06C-56DE-448E-8F1E-6527686E8C73}" name="bad_epoch" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -653,25 +694,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.1796875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="51.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,19 +723,22 @@
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -705,19 +749,22 @@
         <v>601</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -728,19 +775,22 @@
         <v>601</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -751,19 +801,22 @@
         <v>602</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -774,19 +827,22 @@
         <v>602</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -797,19 +853,22 @@
         <v>603</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -820,19 +879,22 @@
         <v>603</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -843,19 +905,22 @@
         <v>605</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -866,19 +931,22 @@
         <v>605</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -888,14 +956,15 @@
       <c r="C10" s="4">
         <v>606</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -905,14 +974,15 @@
       <c r="C11" s="4">
         <v>606</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -923,19 +993,22 @@
         <v>607</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -946,19 +1019,22 @@
         <v>607</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -969,19 +1045,22 @@
         <v>608</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>26</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -992,15 +1071,18 @@
         <v>608</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>18</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor EEG data processing scripts and add README.md for improved clarity and functionality of pipeline
</commit_message>
<xml_diff>
--- a/matlab/subject_data_info.xlsx
+++ b/matlab/subject_data_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/tuna28ng_upenn_edu/Documents/Documents/GitHub/AO_human_v_robot_main/matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="11_F25DC773A252ABDACC1048EAD9DC5C4E5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33FD6B3F-AC75-49DC-B408-5E72640E8566}"/>
+  <xr:revisionPtr revIDLastSave="259" documentId="11_F25DC773A252ABDACC1048EAD9DC5C4E5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29FED975-D311-48B4-8ECA-C44CF81ABA4C}"/>
   <bookViews>
     <workbookView xWindow="-4410" yWindow="-21720" windowWidth="37710" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -412,6 +412,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -697,16 +701,17 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B2" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="95.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="51.140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>

</xml_diff>